<commit_message>
Set datetime colums varchar length to fitting vakue (30 -> 33)
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -6626,7 +6626,7 @@
         <v>83</v>
       </c>
       <c r="F38" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G38" t="n">
         <v>7</v>
@@ -7459,7 +7459,7 @@
         <v>176</v>
       </c>
       <c r="F89" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G89"/>
     </row>
@@ -8227,7 +8227,7 @@
         <v>32</v>
       </c>
       <c r="F137" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G137"/>
     </row>
@@ -8244,7 +8244,7 @@
         <v>32</v>
       </c>
       <c r="F138" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G138"/>
     </row>
@@ -8511,7 +8511,7 @@
         <v>32</v>
       </c>
       <c r="F155" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G155"/>
     </row>
@@ -11119,7 +11119,7 @@
         <v>32</v>
       </c>
       <c r="F315" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G315"/>
     </row>
@@ -14732,7 +14732,7 @@
         <v>32</v>
       </c>
       <c r="F528" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G528"/>
     </row>
@@ -16490,7 +16490,7 @@
         <v>32</v>
       </c>
       <c r="F638" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G638"/>
     </row>
@@ -16541,7 +16541,7 @@
         <v>32</v>
       </c>
       <c r="F641" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G641"/>
     </row>
@@ -19941,7 +19941,7 @@
         <v>32</v>
       </c>
       <c r="F843" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G843"/>
     </row>
@@ -19958,7 +19958,7 @@
         <v>32</v>
       </c>
       <c r="F844" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G844"/>
     </row>
@@ -21968,7 +21968,7 @@
         <v>32</v>
       </c>
       <c r="F968" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G968"/>
     </row>
@@ -21985,7 +21985,7 @@
         <v>32</v>
       </c>
       <c r="F969" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G969"/>
     </row>
@@ -22772,7 +22772,7 @@
         <v>32</v>
       </c>
       <c r="F1020" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G1020"/>
     </row>
@@ -23754,7 +23754,7 @@
         <v>32</v>
       </c>
       <c r="F1084" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G1084"/>
     </row>
@@ -24526,7 +24526,7 @@
         <v>32</v>
       </c>
       <c r="F1132" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G1132"/>
     </row>
@@ -25049,7 +25049,7 @@
         <v>32</v>
       </c>
       <c r="F1165" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G1165"/>
     </row>

</xml_diff>

<commit_message>
Change database string width for datetime from 30 to 35
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -6214,7 +6214,7 @@
         <v>32</v>
       </c>
       <c r="F13" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G13" t="n">
         <v>2</v>
@@ -6233,7 +6233,7 @@
         <v>32</v>
       </c>
       <c r="F14" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G14" t="n">
         <v>2</v>
@@ -6487,7 +6487,7 @@
         <v>32</v>
       </c>
       <c r="F30" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G30"/>
     </row>
@@ -6504,7 +6504,7 @@
         <v>32</v>
       </c>
       <c r="F31" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G31"/>
     </row>
@@ -7346,7 +7346,7 @@
         <v>32</v>
       </c>
       <c r="F83" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G83" t="n">
         <v>2</v>
@@ -7365,7 +7365,7 @@
         <v>32</v>
       </c>
       <c r="F84" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G84" t="n">
         <v>2</v>
@@ -7450,7 +7450,7 @@
         <v>175</v>
       </c>
       <c r="F89" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G89"/>
     </row>
@@ -7676,7 +7676,7 @@
         <v>32</v>
       </c>
       <c r="F103" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G103" t="n">
         <v>2</v>
@@ -7695,7 +7695,7 @@
         <v>32</v>
       </c>
       <c r="F104" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G104" t="n">
         <v>2</v>
@@ -8184,7 +8184,7 @@
         <v>32</v>
       </c>
       <c r="F135" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G135"/>
     </row>
@@ -8201,7 +8201,7 @@
         <v>32</v>
       </c>
       <c r="F136" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G136"/>
     </row>
@@ -8218,7 +8218,7 @@
         <v>32</v>
       </c>
       <c r="F137" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G137"/>
     </row>
@@ -8235,7 +8235,7 @@
         <v>32</v>
       </c>
       <c r="F138" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G138"/>
     </row>
@@ -8329,7 +8329,7 @@
         <v>32</v>
       </c>
       <c r="F144" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G144"/>
     </row>
@@ -8346,7 +8346,7 @@
         <v>32</v>
       </c>
       <c r="F145" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G145"/>
     </row>
@@ -8502,7 +8502,7 @@
         <v>32</v>
       </c>
       <c r="F155" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G155"/>
     </row>
@@ -9282,7 +9282,7 @@
         <v>32</v>
       </c>
       <c r="F203" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G203" t="n">
         <v>2</v>
@@ -9480,7 +9480,7 @@
         <v>32</v>
       </c>
       <c r="F215" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G215" t="n">
         <v>2</v>
@@ -9499,7 +9499,7 @@
         <v>32</v>
       </c>
       <c r="F216" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G216" t="n">
         <v>2</v>
@@ -10470,7 +10470,7 @@
         <v>32</v>
       </c>
       <c r="F275" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G275" t="n">
         <v>2</v>
@@ -10489,7 +10489,7 @@
         <v>32</v>
       </c>
       <c r="F276" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G276" t="n">
         <v>2</v>
@@ -11110,7 +11110,7 @@
         <v>32</v>
       </c>
       <c r="F315" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G315"/>
     </row>
@@ -11823,7 +11823,7 @@
         <v>32</v>
       </c>
       <c r="F358" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G358" t="n">
         <v>2</v>
@@ -11997,7 +11997,7 @@
         <v>32</v>
       </c>
       <c r="F368" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G368" t="n">
         <v>8</v>
@@ -12243,7 +12243,7 @@
         <v>32</v>
       </c>
       <c r="F382" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G382" t="n">
         <v>2</v>
@@ -12262,7 +12262,7 @@
         <v>32</v>
       </c>
       <c r="F383" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G383" t="n">
         <v>2</v>
@@ -12484,7 +12484,7 @@
         <v>727</v>
       </c>
       <c r="F395" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G395" t="n">
         <v>8</v>
@@ -14275,7 +14275,7 @@
         <v>32</v>
       </c>
       <c r="F500" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G500" t="n">
         <v>2</v>
@@ -14294,7 +14294,7 @@
         <v>32</v>
       </c>
       <c r="F501" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G501" t="n">
         <v>2</v>
@@ -14723,7 +14723,7 @@
         <v>32</v>
       </c>
       <c r="F528" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G528"/>
     </row>
@@ -14740,7 +14740,7 @@
         <v>32</v>
       </c>
       <c r="F529" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G529"/>
     </row>
@@ -14757,7 +14757,7 @@
         <v>32</v>
       </c>
       <c r="F530" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G530"/>
     </row>
@@ -15272,7 +15272,7 @@
         <v>32</v>
       </c>
       <c r="F561" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G561" t="n">
         <v>2</v>
@@ -15988,7 +15988,7 @@
         <v>32</v>
       </c>
       <c r="F607" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G607" t="n">
         <v>2</v>
@@ -16007,7 +16007,7 @@
         <v>32</v>
       </c>
       <c r="F608" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G608" t="n">
         <v>2</v>
@@ -16481,7 +16481,7 @@
         <v>32</v>
       </c>
       <c r="F638" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G638"/>
     </row>
@@ -16498,7 +16498,7 @@
         <v>32</v>
       </c>
       <c r="F639" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G639"/>
     </row>
@@ -16515,7 +16515,7 @@
         <v>32</v>
       </c>
       <c r="F640" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G640"/>
     </row>
@@ -16532,7 +16532,7 @@
         <v>32</v>
       </c>
       <c r="F641" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G641"/>
     </row>
@@ -17217,7 +17217,7 @@
         <v>32</v>
       </c>
       <c r="F684" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G684" t="n">
         <v>2</v>
@@ -17391,7 +17391,7 @@
         <v>32</v>
       </c>
       <c r="F694" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G694" t="n">
         <v>8</v>
@@ -17637,7 +17637,7 @@
         <v>32</v>
       </c>
       <c r="F708" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G708" t="n">
         <v>2</v>
@@ -17656,7 +17656,7 @@
         <v>32</v>
       </c>
       <c r="F709" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G709" t="n">
         <v>2</v>
@@ -17878,7 +17878,7 @@
         <v>727</v>
       </c>
       <c r="F721" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G721" t="n">
         <v>8</v>
@@ -19594,7 +19594,7 @@
         <v>32</v>
       </c>
       <c r="F821" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G821" t="n">
         <v>2</v>
@@ -19613,7 +19613,7 @@
         <v>32</v>
       </c>
       <c r="F822" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G822" t="n">
         <v>2</v>
@@ -19932,7 +19932,7 @@
         <v>32</v>
       </c>
       <c r="F843" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G843"/>
     </row>
@@ -19949,7 +19949,7 @@
         <v>32</v>
       </c>
       <c r="F844" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G844"/>
     </row>
@@ -20677,7 +20677,7 @@
         <v>32</v>
       </c>
       <c r="F888" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G888"/>
     </row>
@@ -21726,7 +21726,7 @@
         <v>32</v>
       </c>
       <c r="F953" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G953" t="n">
         <v>2</v>
@@ -21745,7 +21745,7 @@
         <v>32</v>
       </c>
       <c r="F954" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G954" t="n">
         <v>2</v>
@@ -21959,7 +21959,7 @@
         <v>32</v>
       </c>
       <c r="F968" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G968"/>
     </row>
@@ -21976,7 +21976,7 @@
         <v>32</v>
       </c>
       <c r="F969" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G969"/>
     </row>
@@ -22410,7 +22410,7 @@
         <v>32</v>
       </c>
       <c r="F997" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G997" t="n">
         <v>2</v>
@@ -22429,7 +22429,7 @@
         <v>32</v>
       </c>
       <c r="F998" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G998" t="n">
         <v>2</v>
@@ -22763,7 +22763,7 @@
         <v>32</v>
       </c>
       <c r="F1020" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G1020"/>
     </row>
@@ -23332,7 +23332,7 @@
         <v>32</v>
       </c>
       <c r="F1057" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1057" t="n">
         <v>2</v>
@@ -23351,7 +23351,7 @@
         <v>32</v>
       </c>
       <c r="F1058" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1058" t="n">
         <v>2</v>
@@ -23745,7 +23745,7 @@
         <v>32</v>
       </c>
       <c r="F1084" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G1084"/>
     </row>
@@ -23762,7 +23762,7 @@
         <v>32</v>
       </c>
       <c r="F1085" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1085"/>
     </row>
@@ -23779,7 +23779,7 @@
         <v>32</v>
       </c>
       <c r="F1086" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1086"/>
     </row>
@@ -24176,7 +24176,7 @@
         <v>32</v>
       </c>
       <c r="F1111" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1111" t="n">
         <v>2</v>
@@ -24389,7 +24389,7 @@
         <v>32</v>
       </c>
       <c r="F1124" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1124" t="n">
         <v>2</v>
@@ -24408,7 +24408,7 @@
         <v>32</v>
       </c>
       <c r="F1125" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1125" t="n">
         <v>2</v>
@@ -24517,7 +24517,7 @@
         <v>32</v>
       </c>
       <c r="F1132" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G1132"/>
     </row>
@@ -24549,7 +24549,7 @@
         <v>32</v>
       </c>
       <c r="F1134" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1134"/>
     </row>
@@ -24566,7 +24566,7 @@
         <v>32</v>
       </c>
       <c r="F1135" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1135"/>
     </row>
@@ -24733,7 +24733,7 @@
         <v>32</v>
       </c>
       <c r="F1146" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1146"/>
     </row>
@@ -24750,7 +24750,7 @@
         <v>32</v>
       </c>
       <c r="F1147" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1147"/>
     </row>
@@ -24929,7 +24929,7 @@
         <v>32</v>
       </c>
       <c r="F1158" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1158" t="n">
         <v>2</v>
@@ -24948,7 +24948,7 @@
         <v>32</v>
       </c>
       <c r="F1159" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G1159" t="n">
         <v>2</v>
@@ -25040,7 +25040,7 @@
         <v>32</v>
       </c>
       <c r="F1165" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G1165"/>
     </row>

</xml_diff>

<commit_message>
Remove datetime column in pids_per_ward
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="1884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="1883">
   <si>
     <t xml:space="preserve">resource</t>
   </si>
@@ -5655,9 +5655,6 @@
   </si>
   <si>
     <t xml:space="preserve">pids_per_ward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_time</t>
   </si>
   <si>
     <t xml:space="preserve">ward_name</t>
@@ -25036,11 +25033,9 @@
         <v>1881</v>
       </c>
       <c r="D1165"/>
-      <c r="E1165" t="s">
-        <v>32</v>
-      </c>
+      <c r="E1165"/>
       <c r="F1165" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G1165"/>
     </row>
@@ -25055,24 +25050,9 @@
       <c r="D1166"/>
       <c r="E1166"/>
       <c r="F1166" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G1166"/>
-    </row>
-    <row r="1167">
-      <c r="A1167"/>
-      <c r="B1167" t="s">
-        <v>1883</v>
-      </c>
-      <c r="C1167" t="s">
-        <v>1883</v>
-      </c>
-      <c r="D1167"/>
-      <c r="E1167"/>
-      <c r="F1167" t="n">
-        <v>70</v>
-      </c>
-      <c r="G1167"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change TableDescription column names (rename and upper case)
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -26,25 +26,25 @@
     <t xml:space="preserve">'TableDescriptionDefinition' and execute the generation process via the init scripts in the cds2db module.</t>
   </si>
   <si>
-    <t xml:space="preserve">resource</t>
-  </si>
-  <si>
-    <t xml:space="preserve">column_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fhir_expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reference_types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">single_length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">count</t>
+    <t xml:space="preserve">RESOURCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMN_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHIR_EXPRESSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REFERENCE_TYPES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHIR_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SINGLE_LENGTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNT</t>
   </si>
   <si>
     <t xml:space="preserve">Encounter</t>

</xml_diff>

<commit_message>
Fix replace comments in table description definition
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -59,13 +59,13 @@
     <t xml:space="preserve">70</t>
   </si>
   <si>
-    <t xml:space="preserve">enc_patient_id</t>
+    <t xml:space="preserve">enc_patient_ref</t>
   </si>
   <si>
     <t xml:space="preserve">subject/reference</t>
   </si>
   <si>
-    <t xml:space="preserve">enc_partof_id</t>
+    <t xml:space="preserve">enc_partof_ref</t>
   </si>
   <si>
     <t xml:space="preserve">partOf/reference</t>
@@ -263,7 +263,7 @@
     <t xml:space="preserve">period/end</t>
   </si>
   <si>
-    <t xml:space="preserve">enc_diagnosis_condition_id</t>
+    <t xml:space="preserve">enc_diagnosis_condition_ref</t>
   </si>
   <si>
     <t xml:space="preserve">diagnosis/condition/reference</t>
@@ -374,7 +374,7 @@
     <t xml:space="preserve">hospitalization/dischargeDisposition/text</t>
   </si>
   <si>
-    <t xml:space="preserve">enc_location_id</t>
+    <t xml:space="preserve">enc_location_ref</t>
   </si>
   <si>
     <t xml:space="preserve">location/location/reference</t>
@@ -470,7 +470,7 @@
     <t xml:space="preserve">location/location/physicalType/text</t>
   </si>
   <si>
-    <t xml:space="preserve">enc_serviceprovider_id</t>
+    <t xml:space="preserve">enc_serviceprovider_ref</t>
   </si>
   <si>
     <t xml:space="preserve">serviceProvider/reference</t>
@@ -611,13 +611,13 @@
     <t xml:space="preserve">con_id</t>
   </si>
   <si>
-    <t xml:space="preserve">con_encounter_id</t>
+    <t xml:space="preserve">con_encounter_ref</t>
   </si>
   <si>
     <t xml:space="preserve">encounter/reference</t>
   </si>
   <si>
-    <t xml:space="preserve">con_patient_id</t>
+    <t xml:space="preserve">con_patient_ref</t>
   </si>
   <si>
     <t xml:space="preserve">con_identifier_use</t>
@@ -962,7 +962,7 @@
     <t xml:space="preserve">recordedDate</t>
   </si>
   <si>
-    <t xml:space="preserve">con_recorder_id</t>
+    <t xml:space="preserve">con_recorder_ref</t>
   </si>
   <si>
     <t xml:space="preserve">recorder/reference</t>
@@ -1016,7 +1016,7 @@
     <t xml:space="preserve">recorder/display</t>
   </si>
   <si>
-    <t xml:space="preserve">con_asserter_id</t>
+    <t xml:space="preserve">con_asserter_ref</t>
   </si>
   <si>
     <t xml:space="preserve">asserter/reference</t>
@@ -1100,7 +1100,7 @@
     <t xml:space="preserve">stage/summary/text</t>
   </si>
   <si>
-    <t xml:space="preserve">con_stage_assessment_id</t>
+    <t xml:space="preserve">con_stage_assessment_ref</t>
   </si>
   <si>
     <t xml:space="preserve">stage/assessment/reference</t>
@@ -1196,7 +1196,7 @@
     <t xml:space="preserve">note/authorString</t>
   </si>
   <si>
-    <t xml:space="preserve">con_note_authorreference_id</t>
+    <t xml:space="preserve">con_note_authorreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">note/authorReference/reference</t>
@@ -1508,7 +1508,7 @@
     <t xml:space="preserve">ingredient/itemCodeableConcept/text</t>
   </si>
   <si>
-    <t xml:space="preserve">med_ingredient_itemreference_id</t>
+    <t xml:space="preserve">med_ingredient_itemreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">ingredient/itemReference/reference</t>
@@ -1577,10 +1577,10 @@
     <t xml:space="preserve">medreq_id</t>
   </si>
   <si>
-    <t xml:space="preserve">medreq_encounter_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medreq_patient_id</t>
+    <t xml:space="preserve">medreq_encounter_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medreq_patient_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medreq_identifier_use</t>
@@ -1613,7 +1613,7 @@
     <t xml:space="preserve">medreq_identifier_end</t>
   </si>
   <si>
-    <t xml:space="preserve">medreq_medicationreference_id</t>
+    <t xml:space="preserve">medreq_medicationreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medicationReference/reference</t>
@@ -1685,7 +1685,7 @@
     <t xml:space="preserve">reportedBoolean</t>
   </si>
   <si>
-    <t xml:space="preserve">medreq_reportedreference_id</t>
+    <t xml:space="preserve">medreq_reportedreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">reportedReference/reference</t>
@@ -1769,7 +1769,7 @@
     <t xml:space="preserve">medicationCodeableConcept/text</t>
   </si>
   <si>
-    <t xml:space="preserve">medreq_supportinginformation_id</t>
+    <t xml:space="preserve">medreq_supportinginformation_ref</t>
   </si>
   <si>
     <t xml:space="preserve">supportingInformation/reference</t>
@@ -1829,7 +1829,7 @@
     <t xml:space="preserve">authoredOn</t>
   </si>
   <si>
-    <t xml:space="preserve">medreq_requester_id</t>
+    <t xml:space="preserve">medreq_requester_ref</t>
   </si>
   <si>
     <t xml:space="preserve">requester/reference</t>
@@ -1913,7 +1913,7 @@
     <t xml:space="preserve">reasonCode/text</t>
   </si>
   <si>
-    <t xml:space="preserve">medreq_reasonreference_id</t>
+    <t xml:space="preserve">medreq_reasonreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">reasonReference/reference</t>
@@ -1967,7 +1967,7 @@
     <t xml:space="preserve">reasonReference/display</t>
   </si>
   <si>
-    <t xml:space="preserve">medreq_basedon_id</t>
+    <t xml:space="preserve">medreq_basedon_ref</t>
   </si>
   <si>
     <t xml:space="preserve">basedOn/reference</t>
@@ -2024,7 +2024,7 @@
     <t xml:space="preserve">medreq_note_authorstring</t>
   </si>
   <si>
-    <t xml:space="preserve">medreq_note_authorreference_id</t>
+    <t xml:space="preserve">medreq_note_authorreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medreq_note_authorreference_type</t>
@@ -2834,16 +2834,16 @@
     <t xml:space="preserve">medadm_id</t>
   </si>
   <si>
-    <t xml:space="preserve">medadm_encounter_id</t>
+    <t xml:space="preserve">medadm_encounter_ref</t>
   </si>
   <si>
     <t xml:space="preserve">context/reference</t>
   </si>
   <si>
-    <t xml:space="preserve">medadm_patient_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medadm_partof_id</t>
+    <t xml:space="preserve">medadm_patient_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medadm_partof_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medadm_identifier_use</t>
@@ -2909,7 +2909,7 @@
     <t xml:space="preserve">medadm_category_text</t>
   </si>
   <si>
-    <t xml:space="preserve">medadm_medicationreference_id</t>
+    <t xml:space="preserve">medadm_medicationreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medadm_medicationcodeableconcept_system</t>
@@ -2927,7 +2927,7 @@
     <t xml:space="preserve">medadm_medicationcodeableconcept_text</t>
   </si>
   <si>
-    <t xml:space="preserve">medadm_supportinginformation_id</t>
+    <t xml:space="preserve">medadm_supportinginformation_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medadm_supportinginformation_type</t>
@@ -3017,7 +3017,7 @@
     <t xml:space="preserve">medadm_reasoncode_text</t>
   </si>
   <si>
-    <t xml:space="preserve">medadm_reasonreference_id</t>
+    <t xml:space="preserve">medadm_reasonreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medadm_reasonreference_type</t>
@@ -3044,7 +3044,7 @@
     <t xml:space="preserve">medadm_reasonreference_display</t>
   </si>
   <si>
-    <t xml:space="preserve">medadm_request_id</t>
+    <t xml:space="preserve">medadm_request_ref</t>
   </si>
   <si>
     <t xml:space="preserve">request/reference</t>
@@ -3053,7 +3053,7 @@
     <t xml:space="preserve">medadm_note_authorstring</t>
   </si>
   <si>
-    <t xml:space="preserve">medadm_note_authorreference_id</t>
+    <t xml:space="preserve">medadm_note_authorreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medadm_note_authorreference_type</t>
@@ -3326,16 +3326,16 @@
     <t xml:space="preserve">medstat_identifier_end</t>
   </si>
   <si>
-    <t xml:space="preserve">medstat_encounter_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medstat_patient_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medstat_partof_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medstat_basedon_id</t>
+    <t xml:space="preserve">medstat_encounter_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medstat_patient_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medstat_partof_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medstat_basedon_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medstat_basedon_type</t>
@@ -3395,7 +3395,7 @@
     <t xml:space="preserve">medstat_category_text</t>
   </si>
   <si>
-    <t xml:space="preserve">medstat_medicationreference_id</t>
+    <t xml:space="preserve">medstat_medicationreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medstat_medicationcodeableconcept_system</t>
@@ -3428,7 +3428,7 @@
     <t xml:space="preserve">dateAsserted</t>
   </si>
   <si>
-    <t xml:space="preserve">medstat_informationsource_id</t>
+    <t xml:space="preserve">medstat_informationsource_ref</t>
   </si>
   <si>
     <t xml:space="preserve">informationSource/reference</t>
@@ -3482,7 +3482,7 @@
     <t xml:space="preserve">informationSource/display</t>
   </si>
   <si>
-    <t xml:space="preserve">medstat_derivedfrom_id</t>
+    <t xml:space="preserve">medstat_derivedfrom_ref</t>
   </si>
   <si>
     <t xml:space="preserve">derivedFrom/reference</t>
@@ -3551,7 +3551,7 @@
     <t xml:space="preserve">medstat_reasoncode_text</t>
   </si>
   <si>
-    <t xml:space="preserve">medstat_reasonreference_id</t>
+    <t xml:space="preserve">medstat_reasonreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medstat_reasonreference_type</t>
@@ -3581,7 +3581,7 @@
     <t xml:space="preserve">medstat_note_authorstring</t>
   </si>
   <si>
-    <t xml:space="preserve">medstat_note_authorreference_id</t>
+    <t xml:space="preserve">medstat_note_authorreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">medstat_note_authorreference_type</t>
@@ -4304,13 +4304,13 @@
     <t xml:space="preserve">obs_id</t>
   </si>
   <si>
-    <t xml:space="preserve">obs_encounter_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obs_patient_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obs_partof_id</t>
+    <t xml:space="preserve">obs_encounter_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obs_patient_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obs_partof_ref</t>
   </si>
   <si>
     <t xml:space="preserve">obs_identifier_use</t>
@@ -4343,7 +4343,7 @@
     <t xml:space="preserve">obs_identifier_end</t>
   </si>
   <si>
-    <t xml:space="preserve">obs_basedon_id</t>
+    <t xml:space="preserve">obs_basedon_ref</t>
   </si>
   <si>
     <t xml:space="preserve">obs_basedon_type</t>
@@ -4613,7 +4613,7 @@
     <t xml:space="preserve">obs_note_authorstring</t>
   </si>
   <si>
-    <t xml:space="preserve">obs_note_authorreference_id</t>
+    <t xml:space="preserve">obs_note_authorreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">obs_note_authorreference_type</t>
@@ -4676,7 +4676,7 @@
     <t xml:space="preserve">method/text</t>
   </si>
   <si>
-    <t xml:space="preserve">obs_performer_id</t>
+    <t xml:space="preserve">obs_performer_ref</t>
   </si>
   <si>
     <t xml:space="preserve">performer/reference</t>
@@ -4892,7 +4892,7 @@
     <t xml:space="preserve">referenceRange/text</t>
   </si>
   <si>
-    <t xml:space="preserve">obs_hasmember_id</t>
+    <t xml:space="preserve">obs_hasmember_ref</t>
   </si>
   <si>
     <t xml:space="preserve">hasMember/reference</t>
@@ -4952,13 +4952,13 @@
     <t xml:space="preserve">diagrep_id</t>
   </si>
   <si>
-    <t xml:space="preserve">diagrep_encounter_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagrep_patient_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagrep_partof_id</t>
+    <t xml:space="preserve">diagrep_encounter_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagrep_patient_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagrep_partof_ref</t>
   </si>
   <si>
     <t xml:space="preserve">diagrep_identifier_use</t>
@@ -4991,13 +4991,13 @@
     <t xml:space="preserve">diagrep_identifier_end</t>
   </si>
   <si>
-    <t xml:space="preserve">diagrep_result_id</t>
+    <t xml:space="preserve">diagrep_result_ref</t>
   </si>
   <si>
     <t xml:space="preserve">result/reference</t>
   </si>
   <si>
-    <t xml:space="preserve">diagrep_basedon_id</t>
+    <t xml:space="preserve">diagrep_basedon_ref</t>
   </si>
   <si>
     <t xml:space="preserve">diagrep_status</t>
@@ -5039,7 +5039,7 @@
     <t xml:space="preserve">diagrep_issued</t>
   </si>
   <si>
-    <t xml:space="preserve">diagrep_performer_id</t>
+    <t xml:space="preserve">diagrep_performer_ref</t>
   </si>
   <si>
     <t xml:space="preserve">diagrep_performer_type</t>
@@ -5108,10 +5108,10 @@
     <t xml:space="preserve">servreq_id</t>
   </si>
   <si>
-    <t xml:space="preserve">servreq_encounter_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">servreq_patient_id</t>
+    <t xml:space="preserve">servreq_encounter_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">servreq_patient_ref</t>
   </si>
   <si>
     <t xml:space="preserve">servreq_identifier_use</t>
@@ -5144,7 +5144,7 @@
     <t xml:space="preserve">servreq_identifier_end</t>
   </si>
   <si>
-    <t xml:space="preserve">servreq_basedon_id</t>
+    <t xml:space="preserve">servreq_basedon_ref</t>
   </si>
   <si>
     <t xml:space="preserve">servreq_basedon_type</t>
@@ -5213,7 +5213,7 @@
     <t xml:space="preserve">servreq_authoredon</t>
   </si>
   <si>
-    <t xml:space="preserve">servreq_requester_id</t>
+    <t xml:space="preserve">servreq_requester_ref</t>
   </si>
   <si>
     <t xml:space="preserve">servreq_requester_type</t>
@@ -5240,7 +5240,7 @@
     <t xml:space="preserve">servreq_requester_display</t>
   </si>
   <si>
-    <t xml:space="preserve">servreq_performer_id</t>
+    <t xml:space="preserve">servreq_performer_ref</t>
   </si>
   <si>
     <t xml:space="preserve">servreq_performer_type</t>
@@ -5303,13 +5303,13 @@
     <t xml:space="preserve">proc_id</t>
   </si>
   <si>
-    <t xml:space="preserve">proc_encounter_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proc_patient_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proc_partof_id</t>
+    <t xml:space="preserve">proc_encounter_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proc_patient_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proc_partof_ref</t>
   </si>
   <si>
     <t xml:space="preserve">proc_identifier_use</t>
@@ -5342,7 +5342,7 @@
     <t xml:space="preserve">proc_identifier_end</t>
   </si>
   <si>
-    <t xml:space="preserve">proc_basedon_id</t>
+    <t xml:space="preserve">proc_basedon_ref</t>
   </si>
   <si>
     <t xml:space="preserve">proc_basedon_type</t>
@@ -5450,7 +5450,7 @@
     <t xml:space="preserve">proc_reasoncode_text</t>
   </si>
   <si>
-    <t xml:space="preserve">proc_reasonreference_id</t>
+    <t xml:space="preserve">proc_reasonreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">proc_reasonreference_type</t>
@@ -5480,7 +5480,7 @@
     <t xml:space="preserve">proc_note_authorstring</t>
   </si>
   <si>
-    <t xml:space="preserve">proc_note_authorreference_id</t>
+    <t xml:space="preserve">proc_note_authorreference_ref</t>
   </si>
   <si>
     <t xml:space="preserve">proc_note_authorreference_type</t>
@@ -5519,7 +5519,7 @@
     <t xml:space="preserve">cons_id</t>
   </si>
   <si>
-    <t xml:space="preserve">cons_patient_id</t>
+    <t xml:space="preserve">cons_patient_ref</t>
   </si>
   <si>
     <t xml:space="preserve">patient/reference</t>

</xml_diff>

<commit_message>
Fix error for Encounter Class Code FHIR Path in TableDescription
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -164,25 +164,25 @@
     <t xml:space="preserve">enc_class_system</t>
   </si>
   <si>
-    <t xml:space="preserve">class/coding/system</t>
+    <t xml:space="preserve">class/system</t>
   </si>
   <si>
     <t xml:space="preserve">enc_class_version</t>
   </si>
   <si>
-    <t xml:space="preserve">class/coding/version</t>
+    <t xml:space="preserve">class/version</t>
   </si>
   <si>
     <t xml:space="preserve">enc_class_code</t>
   </si>
   <si>
-    <t xml:space="preserve">class/coding/code</t>
+    <t xml:space="preserve">class/code</t>
   </si>
   <si>
     <t xml:space="preserve">enc_class_display</t>
   </si>
   <si>
-    <t xml:space="preserve">class/coding/display</t>
+    <t xml:space="preserve">class/display</t>
   </si>
   <si>
     <t xml:space="preserve">enc_type_system</t>

</xml_diff>

<commit_message>
Fix Encounter Location paths
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -434,7 +434,7 @@
     <t xml:space="preserve">enc_location_status</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/status</t>
+    <t xml:space="preserve">location/status</t>
   </si>
   <si>
     <t xml:space="preserve">10</t>
@@ -443,31 +443,31 @@
     <t xml:space="preserve">enc_location_physicaltype_system</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/physicalType/coding/system</t>
+    <t xml:space="preserve">location/physicalType/coding/system</t>
   </si>
   <si>
     <t xml:space="preserve">enc_location_physicaltype_version</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/physicalType/coding/version</t>
+    <t xml:space="preserve">location/physicalType/coding/version</t>
   </si>
   <si>
     <t xml:space="preserve">enc_location_physicaltype_code</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/physicalType/coding/code</t>
+    <t xml:space="preserve">location/physicalType/coding/code</t>
   </si>
   <si>
     <t xml:space="preserve">enc_location_physicaltype_display</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/physicalType/coding/display</t>
+    <t xml:space="preserve">location/physicalType/coding/display</t>
   </si>
   <si>
     <t xml:space="preserve">enc_location_physicaltype_text</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/physicalType/text</t>
+    <t xml:space="preserve">location/physicalType/text</t>
   </si>
   <si>
     <t xml:space="preserve">enc_serviceprovider_ref</t>

</xml_diff>

<commit_message>
Fix Encounter Location FHIR path
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -434,7 +434,7 @@
     <t xml:space="preserve">enc_location_status</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/status</t>
+    <t xml:space="preserve">location/status</t>
   </si>
   <si>
     <t xml:space="preserve">10</t>
@@ -443,31 +443,31 @@
     <t xml:space="preserve">enc_location_physicaltype_system</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/physicalType/coding/system</t>
+    <t xml:space="preserve">location/physicalType/coding/system</t>
   </si>
   <si>
     <t xml:space="preserve">enc_location_physicaltype_version</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/physicalType/coding/version</t>
+    <t xml:space="preserve">location/physicalType/coding/version</t>
   </si>
   <si>
     <t xml:space="preserve">enc_location_physicaltype_code</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/physicalType/coding/code</t>
+    <t xml:space="preserve">location/physicalType/coding/code</t>
   </si>
   <si>
     <t xml:space="preserve">enc_location_physicaltype_display</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/physicalType/coding/display</t>
+    <t xml:space="preserve">location/physicalType/coding/display</t>
   </si>
   <si>
     <t xml:space="preserve">enc_location_physicaltype_text</t>
   </si>
   <si>
-    <t xml:space="preserve">location/location/physicalType/text</t>
+    <t xml:space="preserve">location/physicalType/text</t>
   </si>
   <si>
     <t xml:space="preserve">enc_serviceprovider_ref</t>

</xml_diff>

<commit_message>
Fix typo in valueCodeableConcept
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -4550,34 +4550,34 @@
     <t xml:space="preserve">valueQuantity/code</t>
   </si>
   <si>
-    <t xml:space="preserve">obs_valuecodableconcept_system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valueCodableConcept/coding/system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obs_valuecodableconcept_version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valueCodableConcept/coding/version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obs_valuecodableconcept_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valueCodableConcept/coding/code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obs_valuecodableconcept_display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valueCodableConcept/coding/display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obs_valuecodableconcept_text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valueCodableConcept/text</t>
+    <t xml:space="preserve">obs_valuecodeableconcept_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valueCodeableConcept/coding/system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obs_valuecodeableconcept_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valueCodeableConcept/coding/version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obs_valuecodeableconcept_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valueCodeableConcept/coding/code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obs_valuecodeableconcept_display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valueCodeableConcept/coding/display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obs_valuecodeableconcept_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valueCodeableConcept/text</t>
   </si>
   <si>
     <t xml:space="preserve">obs_dataabsentreason_system</t>

</xml_diff>

<commit_message>
Add encounter_id column to pids_per_ward database tables
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="1911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="1912">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
@@ -5745,6 +5745,9 @@
   </si>
   <si>
     <t xml:space="preserve">patient_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">encounter_id</t>
   </si>
 </sst>
 </file>
@@ -25191,6 +25194,21 @@
       </c>
       <c r="G1171"/>
     </row>
+    <row r="1172">
+      <c r="A1172"/>
+      <c r="B1172" t="s">
+        <v>1911</v>
+      </c>
+      <c r="C1172" t="s">
+        <v>1911</v>
+      </c>
+      <c r="D1172"/>
+      <c r="E1172"/>
+      <c r="F1172" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1172"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Fix SQL Generator and regenerate
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2057" uniqueCount="2057">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2131" uniqueCount="2131">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
@@ -6071,6 +6071,72 @@
     <t xml:space="preserve">provision/actor/role/text</t>
   </si>
   <si>
+    <t xml:space="preserve">cons_provision_actor_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/actor/reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_actor_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/actor/type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_actor_identifier_use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/actor/identifier/use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_actor_identifier_type_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/actor/identifier/type/coding/system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_actor_identifier_type_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/actor/identifier/type/coding/version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_actor_identifier_type_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/actor/identifier/type/coding/code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_actor_identifier_type_display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/actor/identifier/type/coding/display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_actor_identifier_type_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/actor/identifier/type/text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_actor_identifier_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/actor/identifier/system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_actor_identifier_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/actor/identifier/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_actor_display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/actor/display</t>
+  </si>
+  <si>
     <t xml:space="preserve">cons_provision_code_system</t>
   </si>
   <si>
@@ -6111,6 +6177,162 @@
   </si>
   <si>
     <t xml:space="preserve">provision/dataPeriod/end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_period_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/period/start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_period_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/period/end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_role_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/role/coding/system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_role_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/role/coding/version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_role_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/role/coding/code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_role_display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/role/coding/display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_role_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/role/text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_identifier_use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/identifier/use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_identifier_type_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/identifier/type/coding/system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_identifier_type_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/identifier/type/coding/version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_identifier_type_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/identifier/type/coding/code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_identifier_type_display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/identifier/type/coding/display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_identifier_type_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/identifier/type/text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_identifier_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/identifier/system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_identifier_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/identifier/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_actor_display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/actor/display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_code_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/code/coding/system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_code_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/code/coding/version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_code_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/code/coding/code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_code_display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/code/coding/display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_code_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/code/text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_dataperiod_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/dataPeriod/start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons_provision_provision_dataperiod_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provision/provision/dataPeriod/end</t>
   </si>
   <si>
     <t xml:space="preserve">loc_meta_versionid</t>
@@ -29154,7 +29376,7 @@
       <c r="D1250"/>
       <c r="E1250"/>
       <c r="F1250" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G1250"/>
       <c r="H1250"/>
@@ -29188,7 +29410,7 @@
       <c r="D1252"/>
       <c r="E1252"/>
       <c r="F1252" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G1252"/>
       <c r="H1252"/>
@@ -29205,7 +29427,7 @@
       <c r="D1253"/>
       <c r="E1253"/>
       <c r="F1253" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G1253"/>
       <c r="H1253"/>
@@ -29220,11 +29442,9 @@
         <v>2030</v>
       </c>
       <c r="D1254"/>
-      <c r="E1254" t="s">
-        <v>22</v>
-      </c>
+      <c r="E1254"/>
       <c r="F1254" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G1254"/>
       <c r="H1254"/>
@@ -29239,11 +29459,9 @@
         <v>2032</v>
       </c>
       <c r="D1255"/>
-      <c r="E1255" t="s">
-        <v>22</v>
-      </c>
+      <c r="E1255"/>
       <c r="F1255" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G1255"/>
       <c r="H1255"/>
@@ -29251,24 +29469,28 @@
     </row>
     <row r="1256">
       <c r="A1256"/>
-      <c r="B1256"/>
-      <c r="C1256"/>
+      <c r="B1256" t="s">
+        <v>2033</v>
+      </c>
+      <c r="C1256" t="s">
+        <v>2034</v>
+      </c>
       <c r="D1256"/>
       <c r="E1256"/>
-      <c r="F1256"/>
+      <c r="F1256" t="s">
+        <v>40</v>
+      </c>
       <c r="G1256"/>
       <c r="H1256"/>
       <c r="I1256"/>
     </row>
     <row r="1257">
-      <c r="A1257" t="s">
-        <v>128</v>
-      </c>
+      <c r="A1257"/>
       <c r="B1257" t="s">
-        <v>130</v>
+        <v>2035</v>
       </c>
       <c r="C1257" t="s">
-        <v>15</v>
+        <v>2036</v>
       </c>
       <c r="D1257"/>
       <c r="E1257"/>
@@ -29282,10 +29504,10 @@
     <row r="1258">
       <c r="A1258"/>
       <c r="B1258" t="s">
-        <v>2033</v>
+        <v>2037</v>
       </c>
       <c r="C1258" t="s">
-        <v>18</v>
+        <v>2038</v>
       </c>
       <c r="D1258"/>
       <c r="E1258"/>
@@ -29299,17 +29521,15 @@
     <row r="1259">
       <c r="A1259"/>
       <c r="B1259" t="s">
-        <v>2034</v>
+        <v>2039</v>
       </c>
       <c r="C1259" t="s">
-        <v>21</v>
+        <v>2040</v>
       </c>
       <c r="D1259"/>
-      <c r="E1259" t="s">
-        <v>22</v>
-      </c>
+      <c r="E1259"/>
       <c r="F1259" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G1259"/>
       <c r="H1259"/>
@@ -29318,15 +29538,15 @@
     <row r="1260">
       <c r="A1260"/>
       <c r="B1260" t="s">
-        <v>2035</v>
+        <v>2041</v>
       </c>
       <c r="C1260" t="s">
-        <v>25</v>
+        <v>2042</v>
       </c>
       <c r="D1260"/>
       <c r="E1260"/>
       <c r="F1260" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G1260"/>
       <c r="H1260"/>
@@ -29335,10 +29555,10 @@
     <row r="1261">
       <c r="A1261"/>
       <c r="B1261" t="s">
-        <v>2036</v>
+        <v>2043</v>
       </c>
       <c r="C1261" t="s">
-        <v>28</v>
+        <v>2044</v>
       </c>
       <c r="D1261"/>
       <c r="E1261"/>
@@ -29352,15 +29572,15 @@
     <row r="1262">
       <c r="A1262"/>
       <c r="B1262" t="s">
-        <v>2037</v>
+        <v>2045</v>
       </c>
       <c r="C1262" t="s">
-        <v>31</v>
+        <v>2046</v>
       </c>
       <c r="D1262"/>
       <c r="E1262"/>
       <c r="F1262" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G1262"/>
       <c r="H1262"/>
@@ -29369,15 +29589,15 @@
     <row r="1263">
       <c r="A1263"/>
       <c r="B1263" t="s">
-        <v>2038</v>
+        <v>2047</v>
       </c>
       <c r="C1263" t="s">
-        <v>33</v>
+        <v>2048</v>
       </c>
       <c r="D1263"/>
       <c r="E1263"/>
       <c r="F1263" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G1263"/>
       <c r="H1263"/>
@@ -29386,15 +29606,15 @@
     <row r="1264">
       <c r="A1264"/>
       <c r="B1264" t="s">
-        <v>2039</v>
+        <v>2049</v>
       </c>
       <c r="C1264" t="s">
-        <v>35</v>
+        <v>2050</v>
       </c>
       <c r="D1264"/>
       <c r="E1264"/>
       <c r="F1264" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="G1264"/>
       <c r="H1264"/>
@@ -29403,15 +29623,17 @@
     <row r="1265">
       <c r="A1265"/>
       <c r="B1265" t="s">
-        <v>2040</v>
+        <v>2051</v>
       </c>
       <c r="C1265" t="s">
-        <v>37</v>
+        <v>2052</v>
       </c>
       <c r="D1265"/>
-      <c r="E1265"/>
+      <c r="E1265" t="s">
+        <v>22</v>
+      </c>
       <c r="F1265" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G1265"/>
       <c r="H1265"/>
@@ -29420,15 +29642,17 @@
     <row r="1266">
       <c r="A1266"/>
       <c r="B1266" t="s">
-        <v>2041</v>
+        <v>2053</v>
       </c>
       <c r="C1266" t="s">
-        <v>39</v>
+        <v>2054</v>
       </c>
       <c r="D1266"/>
-      <c r="E1266"/>
+      <c r="E1266" t="s">
+        <v>22</v>
+      </c>
       <c r="F1266" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G1266"/>
       <c r="H1266"/>
@@ -29437,15 +29661,15 @@
     <row r="1267">
       <c r="A1267"/>
       <c r="B1267" t="s">
-        <v>2042</v>
+        <v>2055</v>
       </c>
       <c r="C1267" t="s">
-        <v>42</v>
+        <v>2056</v>
       </c>
       <c r="D1267"/>
       <c r="E1267"/>
       <c r="F1267" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="G1267"/>
       <c r="H1267"/>
@@ -29454,15 +29678,17 @@
     <row r="1268">
       <c r="A1268"/>
       <c r="B1268" t="s">
-        <v>2043</v>
+        <v>2057</v>
       </c>
       <c r="C1268" t="s">
-        <v>44</v>
+        <v>2058</v>
       </c>
       <c r="D1268"/>
-      <c r="E1268"/>
+      <c r="E1268" t="s">
+        <v>22</v>
+      </c>
       <c r="F1268" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G1268"/>
       <c r="H1268"/>
@@ -29471,10 +29697,10 @@
     <row r="1269">
       <c r="A1269"/>
       <c r="B1269" t="s">
-        <v>2044</v>
+        <v>2059</v>
       </c>
       <c r="C1269" t="s">
-        <v>46</v>
+        <v>2060</v>
       </c>
       <c r="D1269"/>
       <c r="E1269" t="s">
@@ -29490,17 +29716,15 @@
     <row r="1270">
       <c r="A1270"/>
       <c r="B1270" t="s">
-        <v>2045</v>
+        <v>2061</v>
       </c>
       <c r="C1270" t="s">
-        <v>48</v>
+        <v>2062</v>
       </c>
       <c r="D1270"/>
-      <c r="E1270" t="s">
-        <v>22</v>
-      </c>
+      <c r="E1270"/>
       <c r="F1270" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G1270"/>
       <c r="H1270"/>
@@ -29509,15 +29733,15 @@
     <row r="1271">
       <c r="A1271"/>
       <c r="B1271" t="s">
-        <v>2046</v>
+        <v>2063</v>
       </c>
       <c r="C1271" t="s">
-        <v>54</v>
+        <v>2064</v>
       </c>
       <c r="D1271"/>
       <c r="E1271"/>
       <c r="F1271" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G1271"/>
       <c r="H1271"/>
@@ -29526,15 +29750,15 @@
     <row r="1272">
       <c r="A1272"/>
       <c r="B1272" t="s">
-        <v>2047</v>
+        <v>2065</v>
       </c>
       <c r="C1272" t="s">
-        <v>2048</v>
+        <v>2066</v>
       </c>
       <c r="D1272"/>
       <c r="E1272"/>
       <c r="F1272" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G1272"/>
       <c r="H1272"/>
@@ -29543,15 +29767,15 @@
     <row r="1273">
       <c r="A1273"/>
       <c r="B1273" t="s">
-        <v>2049</v>
+        <v>2067</v>
       </c>
       <c r="C1273" t="s">
-        <v>2050</v>
+        <v>2068</v>
       </c>
       <c r="D1273"/>
       <c r="E1273"/>
       <c r="F1273" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G1273"/>
       <c r="H1273"/>
@@ -29560,42 +29784,44 @@
     <row r="1274">
       <c r="A1274"/>
       <c r="B1274" t="s">
-        <v>2051</v>
+        <v>2069</v>
       </c>
       <c r="C1274" t="s">
-        <v>2052</v>
+        <v>2070</v>
       </c>
       <c r="D1274"/>
       <c r="E1274"/>
       <c r="F1274" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1274" t="s">
-        <v>74</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="G1274"/>
       <c r="H1274"/>
       <c r="I1274"/>
     </row>
     <row r="1275">
       <c r="A1275"/>
-      <c r="B1275"/>
-      <c r="C1275"/>
+      <c r="B1275" t="s">
+        <v>2071</v>
+      </c>
+      <c r="C1275" t="s">
+        <v>2072</v>
+      </c>
       <c r="D1275"/>
       <c r="E1275"/>
-      <c r="F1275"/>
+      <c r="F1275" t="s">
+        <v>16</v>
+      </c>
       <c r="G1275"/>
       <c r="H1275"/>
       <c r="I1275"/>
     </row>
     <row r="1276">
-      <c r="A1276" t="s">
-        <v>2053</v>
-      </c>
+      <c r="A1276"/>
       <c r="B1276" t="s">
-        <v>2054</v>
+        <v>2073</v>
       </c>
       <c r="C1276" t="s">
-        <v>2054</v>
+        <v>2074</v>
       </c>
       <c r="D1276"/>
       <c r="E1276"/>
@@ -29609,15 +29835,15 @@
     <row r="1277">
       <c r="A1277"/>
       <c r="B1277" t="s">
-        <v>2055</v>
+        <v>2075</v>
       </c>
       <c r="C1277" t="s">
-        <v>2055</v>
+        <v>2076</v>
       </c>
       <c r="D1277"/>
       <c r="E1277"/>
       <c r="F1277" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G1277"/>
       <c r="H1277"/>
@@ -29626,10 +29852,10 @@
     <row r="1278">
       <c r="A1278"/>
       <c r="B1278" t="s">
-        <v>2056</v>
+        <v>2077</v>
       </c>
       <c r="C1278" t="s">
-        <v>2056</v>
+        <v>2078</v>
       </c>
       <c r="D1278"/>
       <c r="E1278"/>
@@ -29639,6 +29865,639 @@
       <c r="G1278"/>
       <c r="H1278"/>
       <c r="I1278"/>
+    </row>
+    <row r="1279">
+      <c r="A1279"/>
+      <c r="B1279" t="s">
+        <v>2079</v>
+      </c>
+      <c r="C1279" t="s">
+        <v>2080</v>
+      </c>
+      <c r="D1279"/>
+      <c r="E1279"/>
+      <c r="F1279" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1279"/>
+      <c r="H1279"/>
+      <c r="I1279"/>
+    </row>
+    <row r="1280">
+      <c r="A1280"/>
+      <c r="B1280" t="s">
+        <v>2081</v>
+      </c>
+      <c r="C1280" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D1280"/>
+      <c r="E1280"/>
+      <c r="F1280" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1280"/>
+      <c r="H1280"/>
+      <c r="I1280"/>
+    </row>
+    <row r="1281">
+      <c r="A1281"/>
+      <c r="B1281" t="s">
+        <v>2083</v>
+      </c>
+      <c r="C1281" t="s">
+        <v>2084</v>
+      </c>
+      <c r="D1281"/>
+      <c r="E1281"/>
+      <c r="F1281" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1281"/>
+      <c r="H1281"/>
+      <c r="I1281"/>
+    </row>
+    <row r="1282">
+      <c r="A1282"/>
+      <c r="B1282" t="s">
+        <v>2085</v>
+      </c>
+      <c r="C1282" t="s">
+        <v>2086</v>
+      </c>
+      <c r="D1282"/>
+      <c r="E1282"/>
+      <c r="F1282" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1282"/>
+      <c r="H1282"/>
+      <c r="I1282"/>
+    </row>
+    <row r="1283">
+      <c r="A1283"/>
+      <c r="B1283" t="s">
+        <v>2087</v>
+      </c>
+      <c r="C1283" t="s">
+        <v>2088</v>
+      </c>
+      <c r="D1283"/>
+      <c r="E1283"/>
+      <c r="F1283" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1283"/>
+      <c r="H1283"/>
+      <c r="I1283"/>
+    </row>
+    <row r="1284">
+      <c r="A1284"/>
+      <c r="B1284" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C1284" t="s">
+        <v>2090</v>
+      </c>
+      <c r="D1284"/>
+      <c r="E1284"/>
+      <c r="F1284" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1284"/>
+      <c r="H1284"/>
+      <c r="I1284"/>
+    </row>
+    <row r="1285">
+      <c r="A1285"/>
+      <c r="B1285" t="s">
+        <v>2091</v>
+      </c>
+      <c r="C1285" t="s">
+        <v>2092</v>
+      </c>
+      <c r="D1285"/>
+      <c r="E1285"/>
+      <c r="F1285" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1285"/>
+      <c r="H1285"/>
+      <c r="I1285"/>
+    </row>
+    <row r="1286">
+      <c r="A1286"/>
+      <c r="B1286" t="s">
+        <v>2093</v>
+      </c>
+      <c r="C1286" t="s">
+        <v>2094</v>
+      </c>
+      <c r="D1286"/>
+      <c r="E1286"/>
+      <c r="F1286" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1286"/>
+      <c r="H1286"/>
+      <c r="I1286"/>
+    </row>
+    <row r="1287">
+      <c r="A1287"/>
+      <c r="B1287" t="s">
+        <v>2095</v>
+      </c>
+      <c r="C1287" t="s">
+        <v>2096</v>
+      </c>
+      <c r="D1287"/>
+      <c r="E1287"/>
+      <c r="F1287" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1287"/>
+      <c r="H1287"/>
+      <c r="I1287"/>
+    </row>
+    <row r="1288">
+      <c r="A1288"/>
+      <c r="B1288" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C1288" t="s">
+        <v>2098</v>
+      </c>
+      <c r="D1288"/>
+      <c r="E1288"/>
+      <c r="F1288" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1288"/>
+      <c r="H1288"/>
+      <c r="I1288"/>
+    </row>
+    <row r="1289">
+      <c r="A1289"/>
+      <c r="B1289" t="s">
+        <v>2099</v>
+      </c>
+      <c r="C1289" t="s">
+        <v>2100</v>
+      </c>
+      <c r="D1289"/>
+      <c r="E1289"/>
+      <c r="F1289" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1289"/>
+      <c r="H1289"/>
+      <c r="I1289"/>
+    </row>
+    <row r="1290">
+      <c r="A1290"/>
+      <c r="B1290" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C1290" t="s">
+        <v>2102</v>
+      </c>
+      <c r="D1290"/>
+      <c r="E1290"/>
+      <c r="F1290" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1290"/>
+      <c r="H1290"/>
+      <c r="I1290"/>
+    </row>
+    <row r="1291">
+      <c r="A1291"/>
+      <c r="B1291" t="s">
+        <v>2103</v>
+      </c>
+      <c r="C1291" t="s">
+        <v>2104</v>
+      </c>
+      <c r="D1291"/>
+      <c r="E1291" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1291" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1291"/>
+      <c r="H1291"/>
+      <c r="I1291"/>
+    </row>
+    <row r="1292">
+      <c r="A1292"/>
+      <c r="B1292" t="s">
+        <v>2105</v>
+      </c>
+      <c r="C1292" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D1292"/>
+      <c r="E1292" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1292" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1292"/>
+      <c r="H1292"/>
+      <c r="I1292"/>
+    </row>
+    <row r="1293">
+      <c r="A1293"/>
+      <c r="B1293"/>
+      <c r="C1293"/>
+      <c r="D1293"/>
+      <c r="E1293"/>
+      <c r="F1293"/>
+      <c r="G1293"/>
+      <c r="H1293"/>
+      <c r="I1293"/>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1294" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1294" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1294"/>
+      <c r="E1294"/>
+      <c r="F1294" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1294"/>
+      <c r="H1294"/>
+      <c r="I1294"/>
+    </row>
+    <row r="1295">
+      <c r="A1295"/>
+      <c r="B1295" t="s">
+        <v>2107</v>
+      </c>
+      <c r="C1295" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1295"/>
+      <c r="E1295"/>
+      <c r="F1295" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1295"/>
+      <c r="H1295"/>
+      <c r="I1295"/>
+    </row>
+    <row r="1296">
+      <c r="A1296"/>
+      <c r="B1296" t="s">
+        <v>2108</v>
+      </c>
+      <c r="C1296" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1296"/>
+      <c r="E1296" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1296" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1296"/>
+      <c r="H1296"/>
+      <c r="I1296"/>
+    </row>
+    <row r="1297">
+      <c r="A1297"/>
+      <c r="B1297" t="s">
+        <v>2109</v>
+      </c>
+      <c r="C1297" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1297"/>
+      <c r="E1297"/>
+      <c r="F1297" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1297"/>
+      <c r="H1297"/>
+      <c r="I1297"/>
+    </row>
+    <row r="1298">
+      <c r="A1298"/>
+      <c r="B1298" t="s">
+        <v>2110</v>
+      </c>
+      <c r="C1298" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1298"/>
+      <c r="E1298"/>
+      <c r="F1298" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1298"/>
+      <c r="H1298"/>
+      <c r="I1298"/>
+    </row>
+    <row r="1299">
+      <c r="A1299"/>
+      <c r="B1299" t="s">
+        <v>2111</v>
+      </c>
+      <c r="C1299" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1299"/>
+      <c r="E1299"/>
+      <c r="F1299" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1299"/>
+      <c r="H1299"/>
+      <c r="I1299"/>
+    </row>
+    <row r="1300">
+      <c r="A1300"/>
+      <c r="B1300" t="s">
+        <v>2112</v>
+      </c>
+      <c r="C1300" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1300"/>
+      <c r="E1300"/>
+      <c r="F1300" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1300"/>
+      <c r="H1300"/>
+      <c r="I1300"/>
+    </row>
+    <row r="1301">
+      <c r="A1301"/>
+      <c r="B1301" t="s">
+        <v>2113</v>
+      </c>
+      <c r="C1301" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1301"/>
+      <c r="E1301"/>
+      <c r="F1301" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1301"/>
+      <c r="H1301"/>
+      <c r="I1301"/>
+    </row>
+    <row r="1302">
+      <c r="A1302"/>
+      <c r="B1302" t="s">
+        <v>2114</v>
+      </c>
+      <c r="C1302" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1302"/>
+      <c r="E1302"/>
+      <c r="F1302" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1302"/>
+      <c r="H1302"/>
+      <c r="I1302"/>
+    </row>
+    <row r="1303">
+      <c r="A1303"/>
+      <c r="B1303" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C1303" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1303"/>
+      <c r="E1303"/>
+      <c r="F1303" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1303"/>
+      <c r="H1303"/>
+      <c r="I1303"/>
+    </row>
+    <row r="1304">
+      <c r="A1304"/>
+      <c r="B1304" t="s">
+        <v>2116</v>
+      </c>
+      <c r="C1304" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1304"/>
+      <c r="E1304"/>
+      <c r="F1304" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1304"/>
+      <c r="H1304"/>
+      <c r="I1304"/>
+    </row>
+    <row r="1305">
+      <c r="A1305"/>
+      <c r="B1305" t="s">
+        <v>2117</v>
+      </c>
+      <c r="C1305" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1305"/>
+      <c r="E1305"/>
+      <c r="F1305" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1305"/>
+      <c r="H1305"/>
+      <c r="I1305"/>
+    </row>
+    <row r="1306">
+      <c r="A1306"/>
+      <c r="B1306" t="s">
+        <v>2118</v>
+      </c>
+      <c r="C1306" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1306"/>
+      <c r="E1306" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1306" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1306"/>
+      <c r="H1306"/>
+      <c r="I1306"/>
+    </row>
+    <row r="1307">
+      <c r="A1307"/>
+      <c r="B1307" t="s">
+        <v>2119</v>
+      </c>
+      <c r="C1307" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1307"/>
+      <c r="E1307" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1307" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1307"/>
+      <c r="H1307"/>
+      <c r="I1307"/>
+    </row>
+    <row r="1308">
+      <c r="A1308"/>
+      <c r="B1308" t="s">
+        <v>2120</v>
+      </c>
+      <c r="C1308" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1308"/>
+      <c r="E1308"/>
+      <c r="F1308" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1308"/>
+      <c r="H1308"/>
+      <c r="I1308"/>
+    </row>
+    <row r="1309">
+      <c r="A1309"/>
+      <c r="B1309" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C1309" t="s">
+        <v>2122</v>
+      </c>
+      <c r="D1309"/>
+      <c r="E1309"/>
+      <c r="F1309" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1309"/>
+      <c r="H1309"/>
+      <c r="I1309"/>
+    </row>
+    <row r="1310">
+      <c r="A1310"/>
+      <c r="B1310" t="s">
+        <v>2123</v>
+      </c>
+      <c r="C1310" t="s">
+        <v>2124</v>
+      </c>
+      <c r="D1310"/>
+      <c r="E1310"/>
+      <c r="F1310" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1310"/>
+      <c r="H1310"/>
+      <c r="I1310"/>
+    </row>
+    <row r="1311">
+      <c r="A1311"/>
+      <c r="B1311" t="s">
+        <v>2125</v>
+      </c>
+      <c r="C1311" t="s">
+        <v>2126</v>
+      </c>
+      <c r="D1311"/>
+      <c r="E1311"/>
+      <c r="F1311" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1311" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1311"/>
+      <c r="I1311"/>
+    </row>
+    <row r="1312">
+      <c r="A1312"/>
+      <c r="B1312"/>
+      <c r="C1312"/>
+      <c r="D1312"/>
+      <c r="E1312"/>
+      <c r="F1312"/>
+      <c r="G1312"/>
+      <c r="H1312"/>
+      <c r="I1312"/>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="s">
+        <v>2127</v>
+      </c>
+      <c r="B1313" t="s">
+        <v>2128</v>
+      </c>
+      <c r="C1313" t="s">
+        <v>2128</v>
+      </c>
+      <c r="D1313"/>
+      <c r="E1313"/>
+      <c r="F1313" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1313"/>
+      <c r="H1313"/>
+      <c r="I1313"/>
+    </row>
+    <row r="1314">
+      <c r="A1314"/>
+      <c r="B1314" t="s">
+        <v>2129</v>
+      </c>
+      <c r="C1314" t="s">
+        <v>2129</v>
+      </c>
+      <c r="D1314"/>
+      <c r="E1314"/>
+      <c r="F1314" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1314"/>
+      <c r="H1314"/>
+      <c r="I1314"/>
+    </row>
+    <row r="1315">
+      <c r="A1315"/>
+      <c r="B1315" t="s">
+        <v>2130</v>
+      </c>
+      <c r="C1315" t="s">
+        <v>2130</v>
+      </c>
+      <c r="D1315"/>
+      <c r="E1315"/>
+      <c r="F1315" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1315"/>
+      <c r="H1315"/>
+      <c r="I1315"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Location physicalType in db
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2131" uniqueCount="2131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2141" uniqueCount="2141">
   <si>
     <t xml:space="preserve">Hint</t>
   </si>
@@ -6393,6 +6393,36 @@
   </si>
   <si>
     <t xml:space="preserve">alias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc_physicaltype_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">physicalType/coding/system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc_physicaltype_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">physicalType/coding/version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc_physicaltype_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">physicalType/coding/code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc_physicaltype_display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">physicalType/coding/display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc_physicaltype_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">physicalType/text</t>
   </si>
   <si>
     <t xml:space="preserve">pids_per_ward</t>
@@ -30437,29 +30467,33 @@
     </row>
     <row r="1312">
       <c r="A1312"/>
-      <c r="B1312"/>
-      <c r="C1312"/>
+      <c r="B1312" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C1312" t="s">
+        <v>2128</v>
+      </c>
       <c r="D1312"/>
       <c r="E1312"/>
-      <c r="F1312"/>
+      <c r="F1312" t="s">
+        <v>16</v>
+      </c>
       <c r="G1312"/>
       <c r="H1312"/>
       <c r="I1312"/>
     </row>
     <row r="1313">
-      <c r="A1313" t="s">
-        <v>2127</v>
-      </c>
+      <c r="A1313"/>
       <c r="B1313" t="s">
-        <v>2128</v>
+        <v>2129</v>
       </c>
       <c r="C1313" t="s">
-        <v>2128</v>
+        <v>2130</v>
       </c>
       <c r="D1313"/>
       <c r="E1313"/>
       <c r="F1313" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G1313"/>
       <c r="H1313"/>
@@ -30468,15 +30502,15 @@
     <row r="1314">
       <c r="A1314"/>
       <c r="B1314" t="s">
-        <v>2129</v>
+        <v>2131</v>
       </c>
       <c r="C1314" t="s">
-        <v>2129</v>
+        <v>2132</v>
       </c>
       <c r="D1314"/>
       <c r="E1314"/>
       <c r="F1314" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G1314"/>
       <c r="H1314"/>
@@ -30485,19 +30519,100 @@
     <row r="1315">
       <c r="A1315"/>
       <c r="B1315" t="s">
-        <v>2130</v>
+        <v>2133</v>
       </c>
       <c r="C1315" t="s">
-        <v>2130</v>
+        <v>2134</v>
       </c>
       <c r="D1315"/>
       <c r="E1315"/>
       <c r="F1315" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G1315"/>
       <c r="H1315"/>
       <c r="I1315"/>
+    </row>
+    <row r="1316">
+      <c r="A1316"/>
+      <c r="B1316" t="s">
+        <v>2135</v>
+      </c>
+      <c r="C1316" t="s">
+        <v>2136</v>
+      </c>
+      <c r="D1316"/>
+      <c r="E1316"/>
+      <c r="F1316" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1316"/>
+      <c r="H1316"/>
+      <c r="I1316"/>
+    </row>
+    <row r="1317">
+      <c r="A1317"/>
+      <c r="B1317"/>
+      <c r="C1317"/>
+      <c r="D1317"/>
+      <c r="E1317"/>
+      <c r="F1317"/>
+      <c r="G1317"/>
+      <c r="H1317"/>
+      <c r="I1317"/>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="s">
+        <v>2137</v>
+      </c>
+      <c r="B1318" t="s">
+        <v>2138</v>
+      </c>
+      <c r="C1318" t="s">
+        <v>2138</v>
+      </c>
+      <c r="D1318"/>
+      <c r="E1318"/>
+      <c r="F1318" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1318"/>
+      <c r="H1318"/>
+      <c r="I1318"/>
+    </row>
+    <row r="1319">
+      <c r="A1319"/>
+      <c r="B1319" t="s">
+        <v>2139</v>
+      </c>
+      <c r="C1319" t="s">
+        <v>2139</v>
+      </c>
+      <c r="D1319"/>
+      <c r="E1319"/>
+      <c r="F1319" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1319"/>
+      <c r="H1319"/>
+      <c r="I1319"/>
+    </row>
+    <row r="1320">
+      <c r="A1320"/>
+      <c r="B1320" t="s">
+        <v>2140</v>
+      </c>
+      <c r="C1320" t="s">
+        <v>2140</v>
+      </c>
+      <c r="D1320"/>
+      <c r="E1320"/>
+      <c r="F1320" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1320"/>
+      <c r="H1320"/>
+      <c r="I1320"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Table_Description with Medication self reference
</commit_message>
<xml_diff>
--- a/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
+++ b/R-cds2db/cds2db/inst/extdata/Table_Description.xlsx
@@ -10539,10 +10539,16 @@
       <c r="C288" t="s">
         <v>529</v>
       </c>
-      <c r="D288"/>
+      <c r="D288" t="s">
+        <v>447</v>
+      </c>
       <c r="E288"/>
-      <c r="F288"/>
-      <c r="G288"/>
+      <c r="F288" t="s">
+        <v>448</v>
+      </c>
+      <c r="G288" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289"/>

</xml_diff>